<commit_message>
first draft of nov 2022
</commit_message>
<xml_diff>
--- a/docs/psy/file08_sound/defineTrials.xlsx
+++ b/docs/psy/file08_sound/defineTrials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgreen\gits\psychopy-training-1-of-2\psy\file8_sound\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgreen\gits\psychopy-training-1-of-2\psy\file08_sound\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3141F8FC-90D7-476F-B25B-3FDC95F8B099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876AAA74-DF8C-479F-883C-29E948151DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCE04B16-6D1C-451A-9FC4-CE9ADB92DB36}"/>
+    <workbookView xWindow="1125" yWindow="-15075" windowWidth="21600" windowHeight="11385" xr2:uid="{DCE04B16-6D1C-451A-9FC4-CE9ADB92DB36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,13 +85,13 @@
     <t>human</t>
   </si>
   <si>
-    <t>musical tone</t>
-  </si>
-  <si>
     <t>thunderstorm.wav</t>
   </si>
   <si>
     <t>cafe.ogg</t>
+  </si>
+  <si>
+    <t>nature</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -501,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -518,7 +518,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -535,7 +535,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -552,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -569,10 +569,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -586,10 +586,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -603,10 +603,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -620,10 +620,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -637,10 +637,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>

</xml_diff>